<commit_message>
update images and readme
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dbb3bcb016510c61/Dokumente/GitHub/SolderCase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dbb3bcb016510c61/MLR/Projekte/_GitHub/SolderCase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="242" documentId="8_{C04FB23A-8B55-4235-BABD-929EC625D60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83F6082F-F3B7-4829-AB3A-E485C952F1A1}"/>
+  <xr:revisionPtr revIDLastSave="245" documentId="8_{C04FB23A-8B55-4235-BABD-929EC625D60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4428CC27-8F17-4E6E-890E-53F21D87BBF1}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{A69D1F71-165B-4D0C-BF55-3E1746EE05B2}"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="10590" windowHeight="6922" xr2:uid="{A69D1F71-165B-4D0C-BF55-3E1746EE05B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>#</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Pinecil</t>
   </si>
   <si>
-    <t>SUMME</t>
-  </si>
-  <si>
     <t>PC fan, 120mm, ca. 25mm thick, 24V</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>ferrule 0,75mm^2</t>
   </si>
   <si>
-    <t>cable lug 0,75mm^2</t>
-  </si>
-  <si>
     <t>MDF wood, 3mm, 570x500 mm</t>
   </si>
   <si>
@@ -160,6 +154,9 @@
   </si>
   <si>
     <t>zip tie, 15cm</t>
+  </si>
+  <si>
+    <t>cable lug 0,75mm^2, two small, four medium</t>
   </si>
 </sst>
 </file>
@@ -597,8 +594,8 @@
   </sheetPr>
   <dimension ref="B1:S76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -616,27 +613,27 @@
     </row>
     <row r="4" spans="2:19" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:19" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="S5" s="10"/>
     </row>
@@ -648,7 +645,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5">
         <v>4</v>
@@ -670,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" s="5">
         <v>3.72</v>
@@ -692,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="5">
         <f>5.25/10</f>
@@ -716,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="5">
         <f>1.55/5</f>
@@ -740,7 +737,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E10" s="5">
         <f>8.99/40</f>
@@ -764,7 +761,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="5">
         <f>8.49/12</f>
@@ -788,7 +785,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="5">
         <f>10.5/5</f>
@@ -835,7 +832,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="5">
         <v>3.84</v>
@@ -858,7 +855,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E15" s="5">
         <v>3.99</v>
@@ -881,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="5">
         <f>3.4/3</f>
@@ -905,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" s="5">
         <v>1.78</v>
@@ -928,7 +925,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="5">
         <v>1.56</v>
@@ -951,7 +948,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E19" s="5">
         <v>6.9</v>
@@ -974,7 +971,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" s="5">
         <f>18.5/12</f>
@@ -998,7 +995,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>
@@ -1020,7 +1017,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" s="5">
         <f>13.95/100</f>
@@ -1043,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23" s="5">
         <f>9.99/20</f>
@@ -1066,7 +1063,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E24" s="5">
         <v>16</v>
@@ -1088,7 +1085,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E25" s="5">
         <v>12.5</v>
@@ -1110,7 +1107,7 @@
         <v>8</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E26" s="5">
         <v>0</v>
@@ -1128,7 +1125,7 @@
         <v>8</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E27" s="5">
         <v>0</v>
@@ -1146,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E28" s="5">
         <v>0</v>
@@ -1164,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E29" s="5">
         <v>0</v>
@@ -1182,7 +1179,7 @@
         <v>4</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E30" s="5">
         <v>0</v>
@@ -1200,7 +1197,7 @@
         <v>2</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E31" s="5">
         <v>0</v>
@@ -1218,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E32" s="5">
         <v>0</v>
@@ -1236,7 +1233,7 @@
         <v>1</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E33" s="5">
         <v>0</v>
@@ -1254,7 +1251,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E34" s="5">
         <v>0</v>
@@ -1272,7 +1269,7 @@
         <v>5</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E35" s="5">
         <v>0</v>
@@ -1287,10 +1284,10 @@
         <v>31</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E36" s="5">
         <v>0</v>
@@ -1308,7 +1305,7 @@
         <v>2</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E37" s="5">
         <v>0</v>
@@ -1326,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E38" s="5">
         <v>0</v>
@@ -1338,7 +1335,7 @@
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.45">
       <c r="D39" s="16" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="F39" s="7">
         <f>SUM(F6:F36)</f>

</xml_diff>